<commit_message>
Added cast to the sheet, only 1st 5 actors
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Genres" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$Q$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$R$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Rating</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -714,13 +720,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,18 +737,20 @@
     <col min="4" max="4" width="75.42578125" style="9" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="44.140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="20.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="20.85546875" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="50" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="64.7109375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="25.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="28.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="47.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.28515625" style="11" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.140625" style="11"/>
+    <col min="7" max="7" width="32.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.28515625" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="20.85546875" style="9" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="50" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="64.7109375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="25.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="28.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="47.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" style="11" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.140625" style="11" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>71</v>
       </c>
@@ -762,40 +770,43 @@
         <v>74</v>
       </c>
       <c r="G1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -804,20 +815,22 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="E2" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="18"/>
+      <c r="J2" s="11"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="18"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -826,20 +839,22 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="18"/>
+      <c r="J3" s="11"/>
+      <c r="L3" s="8"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="18"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -848,20 +863,22 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="E4" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="18"/>
+      <c r="J4" s="11"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="18"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -870,20 +887,23 @@
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
+      <c r="E5" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="F5" s="18"/>
-      <c r="G5" s="11"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="18"/>
+      <c r="J5" s="11"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="18"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -892,20 +912,22 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="18"/>
+      <c r="J6" s="11"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -914,21 +936,23 @@
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="18"/>
+      <c r="J7" s="11"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q8"/>
+  <autoFilter ref="A1:R8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added subfolder column, improved testing, design
</commit_message>
<xml_diff>
--- a/movies.xlsx
+++ b/movies.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Genres" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$R$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Moviebase!$A$1:$S$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Rating</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Subfolder</t>
   </si>
 </sst>
 </file>
@@ -720,13 +723,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,23 +737,24 @@
     <col min="1" max="1" width="51.85546875" style="7" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="7.28515625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.42578125" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="75.42578125" style="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.5703125" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.28515625" style="9" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="20.85546875" style="9" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="50" style="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="64.7109375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="25.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="28.85546875" style="11" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="47.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.28515625" style="11" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.140625" style="11" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="44.140625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.5703125" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.28515625" style="9" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="20.85546875" style="9" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.140625" style="6" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="50" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="64.7109375" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="25.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="28.85546875" style="11" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="47.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.28515625" style="11" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="11" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>71</v>
       </c>
@@ -760,53 +764,56 @@
       <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -814,23 +821,24 @@
         <v>2019</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="18"/>
+      <c r="K2" s="11"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
       <c r="R2" s="18"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="18"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -838,23 +846,24 @@
         <v>2018</v>
       </c>
       <c r="C3" s="7"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="G3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="18"/>
+      <c r="K3" s="11"/>
+      <c r="M3" s="8"/>
       <c r="N3" s="18"/>
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="18"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -862,23 +871,24 @@
         <v>1995</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="18"/>
+      <c r="K4" s="11"/>
+      <c r="M4" s="8"/>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="18"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
@@ -886,24 +896,25 @@
         <v>2017</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="18"/>
+      <c r="K5" s="11"/>
+      <c r="M5" s="8"/>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="18"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -911,23 +922,24 @@
         <v>2021</v>
       </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="18"/>
+      <c r="K6" s="11"/>
+      <c r="M6" s="8"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
       <c r="R6" s="18"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="18"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
@@ -935,24 +947,25 @@
         <v>1993</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="18"/>
+      <c r="K7" s="11"/>
+      <c r="M7" s="8"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R8"/>
+  <autoFilter ref="A1:S8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>